<commit_message>
Haven't done this in a while
</commit_message>
<xml_diff>
--- a/XLSXExample.xlsx
+++ b/XLSXExample.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Name (Last, First)</t>
   </si>
@@ -73,9 +73,6 @@
   </si>
   <si>
     <t>Zero</t>
-  </si>
-  <si>
-    <t>5, Johnny</t>
   </si>
   <si>
     <t>McCraken, Rex</t>
@@ -414,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D3"/>
+      <selection activeCell="A18" sqref="A18:XFD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -443,7 +440,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="1">
-        <v>123</v>
+        <v>85436</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -451,7 +448,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="1">
-        <v>456</v>
+        <v>27056</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -571,7 +568,7 @@
         <v>19</v>
       </c>
       <c r="B18" s="1">
-        <v>5</v>
+        <v>1234</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -579,14 +576,6 @@
         <v>20</v>
       </c>
       <c r="B19" s="1">
-        <v>1234</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20" s="1">
         <v>345</v>
       </c>
     </row>

</xml_diff>